<commit_message>
Add tournament results for Seasons 1 and 2
</commit_message>
<xml_diff>
--- a/data/Rivals1Tournaments.xlsx
+++ b/data/Rivals1Tournaments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlmon\Documents\GitHub\rivals-blog\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA397E6-36A2-4B71-BA38-7C5FE45B25CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEC0A56-C1F1-435A-8CD4-8172B4B6B7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2A244B74-61B1-45DC-BA53-937AAD983688}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{2A244B74-61B1-45DC-BA53-937AAD983688}"/>
   </bookViews>
   <sheets>
     <sheet name="Season 1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="394">
   <si>
     <t>Name</t>
   </si>
@@ -917,16 +917,331 @@
   </si>
   <si>
     <t>AppleWiz</t>
+  </si>
+  <si>
+    <t>Road to Shine: Rivals</t>
+  </si>
+  <si>
+    <t>The Bigger Balc</t>
+  </si>
+  <si>
+    <t>Pomona, CA</t>
+  </si>
+  <si>
+    <t>NA RCS July Monthly</t>
+  </si>
+  <si>
+    <t>Low Tier City 5</t>
+  </si>
+  <si>
+    <t>Irving, TX</t>
+  </si>
+  <si>
+    <t>Rivals @ Super Smash Con</t>
+  </si>
+  <si>
+    <t>NA RCS August Monthly</t>
+  </si>
+  <si>
+    <t>Shine 2017</t>
+  </si>
+  <si>
+    <t>NA RCS September Monthly</t>
+  </si>
+  <si>
+    <t>Heat Wave</t>
+  </si>
+  <si>
+    <t>GameTyrant Expo 2017</t>
+  </si>
+  <si>
+    <t>Salt Lake City, UT</t>
+  </si>
+  <si>
+    <t>NA RCS October Monthly</t>
+  </si>
+  <si>
+    <t>NA RCS November Monthly</t>
+  </si>
+  <si>
+    <t>NA RCS December Monthly</t>
+  </si>
+  <si>
+    <t>Genesis 5</t>
+  </si>
+  <si>
+    <t>Genesis 4</t>
+  </si>
+  <si>
+    <t>Rewired 2016</t>
+  </si>
+  <si>
+    <t>Shine 2016</t>
+  </si>
+  <si>
+    <t>Smash Summit 3</t>
+  </si>
+  <si>
+    <t>NA RCS Week 1</t>
+  </si>
+  <si>
+    <t>NA RCS Week 2</t>
+  </si>
+  <si>
+    <t>NA RCS Week 3</t>
+  </si>
+  <si>
+    <t>NA RCS Week 4</t>
+  </si>
+  <si>
+    <t>NA RCS Week 5</t>
+  </si>
+  <si>
+    <t>NA RCS Week 6</t>
+  </si>
+  <si>
+    <t>NA RCS Week 7</t>
+  </si>
+  <si>
+    <t>NA RCS Week 8</t>
+  </si>
+  <si>
+    <t>NA RCS Week 9</t>
+  </si>
+  <si>
+    <t>NA RCS Week 10</t>
+  </si>
+  <si>
+    <t>NA RCS Week 11</t>
+  </si>
+  <si>
+    <t>NA RCS Week 12</t>
+  </si>
+  <si>
+    <t>Garden of Gods - A Rivals of Aether National</t>
+  </si>
+  <si>
+    <t>GUTS 4 Game Underground Tournament Spectacular 4</t>
+  </si>
+  <si>
+    <t>Kennesaw, GA</t>
+  </si>
+  <si>
+    <t>Ledyard, CT</t>
+  </si>
+  <si>
+    <t>Tucson, AZ</t>
+  </si>
+  <si>
+    <t>MrLz</t>
+  </si>
+  <si>
+    <t>PikaThePikachu</t>
+  </si>
+  <si>
+    <t>TheFailWhale1</t>
+  </si>
+  <si>
+    <t>Guyron</t>
+  </si>
+  <si>
+    <t>Ralph</t>
+  </si>
+  <si>
+    <t>Risky</t>
+  </si>
+  <si>
+    <t>Quote_a</t>
+  </si>
+  <si>
+    <t>Golden Elite</t>
+  </si>
+  <si>
+    <t>Bicycle</t>
+  </si>
+  <si>
+    <t>Turquoise</t>
+  </si>
+  <si>
+    <t>Zantoma</t>
+  </si>
+  <si>
+    <t>Dank Fornasty</t>
+  </si>
+  <si>
+    <t>alexis</t>
+  </si>
+  <si>
+    <t>Stan Fornace</t>
+  </si>
+  <si>
+    <t>Wigg</t>
+  </si>
+  <si>
+    <t>Fatty Jabbers</t>
+  </si>
+  <si>
+    <t>Egman</t>
+  </si>
+  <si>
+    <t>Kalvar</t>
+  </si>
+  <si>
+    <t>DJ</t>
+  </si>
+  <si>
+    <t>Dirtydan</t>
+  </si>
+  <si>
+    <t>Enetick</t>
+  </si>
+  <si>
+    <t>Twin</t>
+  </si>
+  <si>
+    <t>「DIO」</t>
+  </si>
+  <si>
+    <t>Coach Hines</t>
+  </si>
+  <si>
+    <t>TheDuoDesign</t>
+  </si>
+  <si>
+    <t>Phuege</t>
+  </si>
+  <si>
+    <t>Shengon</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Cluf</t>
+  </si>
+  <si>
+    <t>RK987</t>
+  </si>
+  <si>
+    <t>Kaos</t>
+  </si>
+  <si>
+    <t>CEO: Dreamland</t>
+  </si>
+  <si>
+    <t>Orlando, FL</t>
+  </si>
+  <si>
+    <t>Aurecia</t>
+  </si>
+  <si>
+    <t>Renzo</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Rivals of Aether @ TwitchCon</t>
+  </si>
+  <si>
+    <t>San Diego, CA</t>
+  </si>
+  <si>
+    <t>Shinku</t>
+  </si>
+  <si>
+    <t>serioussarcasm</t>
+  </si>
+  <si>
+    <t>TheBestAdamCarra</t>
+  </si>
+  <si>
+    <t>Mista J</t>
+  </si>
+  <si>
+    <t>LiBrizzi</t>
+  </si>
+  <si>
+    <t>RiskyCB</t>
+  </si>
+  <si>
+    <t>Los Angeles, CA</t>
+  </si>
+  <si>
+    <t>Mang0</t>
+  </si>
+  <si>
+    <t>Plup</t>
+  </si>
+  <si>
+    <t>Axe</t>
+  </si>
+  <si>
+    <t>Shroomed</t>
+  </si>
+  <si>
+    <t>Hungrybox</t>
+  </si>
+  <si>
+    <t>SFAT</t>
+  </si>
+  <si>
+    <t>Westballz</t>
+  </si>
+  <si>
+    <t>The Moon</t>
+  </si>
+  <si>
+    <t>TheEvets</t>
+  </si>
+  <si>
+    <t>Heyodogo</t>
+  </si>
+  <si>
+    <t>IT’S A CAT :D</t>
+  </si>
+  <si>
+    <t>Youngblood</t>
+  </si>
+  <si>
+    <t>Skittles</t>
+  </si>
+  <si>
+    <t>Mephiles</t>
+  </si>
+  <si>
+    <t>Handbuttt</t>
+  </si>
+  <si>
+    <t>gracefulknight</t>
+  </si>
+  <si>
+    <t>Toko</t>
+  </si>
+  <si>
+    <t>Etalus</t>
+  </si>
+  <si>
+    <t>Rato</t>
+  </si>
+  <si>
+    <t>Shadow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1289,26 +1604,1666 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283BCD14-DCE6-4889-BB2A-A11A8BE83845}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView zoomScale="66" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B2">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1">
+        <v>42644</v>
+      </c>
+      <c r="F2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" t="s">
+        <v>329</v>
+      </c>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" t="s">
+        <v>330</v>
+      </c>
+      <c r="M2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B3">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1">
+        <v>42651</v>
+      </c>
+      <c r="F3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" t="s">
+        <v>333</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" t="s">
+        <v>329</v>
+      </c>
+      <c r="K3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B4">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42658</v>
+      </c>
+      <c r="F4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" t="s">
+        <v>329</v>
+      </c>
+      <c r="I4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" t="s">
+        <v>331</v>
+      </c>
+      <c r="K4" t="s">
+        <v>138</v>
+      </c>
+      <c r="L4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B5">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1">
+        <v>42665</v>
+      </c>
+      <c r="F5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>331</v>
+      </c>
+      <c r="J5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" t="s">
+        <v>336</v>
+      </c>
+      <c r="M5" t="s">
+        <v>337</v>
+      </c>
+      <c r="N5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B6">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>326</v>
+      </c>
+      <c r="E6" s="1">
+        <v>42665</v>
+      </c>
+      <c r="F6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>338</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" t="s">
+        <v>334</v>
+      </c>
+      <c r="K6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" t="s">
+        <v>183</v>
+      </c>
+      <c r="N6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>316</v>
+      </c>
+      <c r="B7">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1">
+        <v>42672</v>
+      </c>
+      <c r="F7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>330</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" t="s">
+        <v>335</v>
+      </c>
+      <c r="L7" t="s">
+        <v>334</v>
+      </c>
+      <c r="M7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>317</v>
+      </c>
+      <c r="B8">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1">
+        <v>42679</v>
+      </c>
+      <c r="F8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" t="s">
+        <v>333</v>
+      </c>
+      <c r="H8" t="s">
+        <v>340</v>
+      </c>
+      <c r="I8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" t="s">
+        <v>329</v>
+      </c>
+      <c r="L8" t="s">
+        <v>331</v>
+      </c>
+      <c r="M8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>325</v>
+      </c>
+      <c r="B9">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>327</v>
+      </c>
+      <c r="E9" s="1">
+        <v>42685</v>
+      </c>
+      <c r="F9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" t="s">
+        <v>340</v>
+      </c>
+      <c r="H9" t="s">
+        <v>341</v>
+      </c>
+      <c r="I9" t="s">
+        <v>342</v>
+      </c>
+      <c r="J9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K9" t="s">
+        <v>344</v>
+      </c>
+      <c r="L9" t="s">
+        <v>345</v>
+      </c>
+      <c r="M9" t="s">
+        <v>346</v>
+      </c>
+      <c r="N9" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>318</v>
+      </c>
+      <c r="B10">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1">
+        <v>42686</v>
+      </c>
+      <c r="F10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G10" t="s">
+        <v>333</v>
+      </c>
+      <c r="H10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" t="s">
+        <v>331</v>
+      </c>
+      <c r="K10" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>309</v>
+      </c>
+      <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>328</v>
+      </c>
+      <c r="E11" s="1">
+        <v>42692</v>
+      </c>
+      <c r="F11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" t="s">
+        <v>329</v>
+      </c>
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" t="s">
+        <v>183</v>
+      </c>
+      <c r="J11" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" t="s">
+        <v>348</v>
+      </c>
+      <c r="L11" t="s">
+        <v>349</v>
+      </c>
+      <c r="M11" t="s">
+        <v>350</v>
+      </c>
+      <c r="N11" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>319</v>
+      </c>
+      <c r="B12">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1">
+        <v>42693</v>
+      </c>
+      <c r="F12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" t="s">
+        <v>340</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M12" t="s">
+        <v>331</v>
+      </c>
+      <c r="N12" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>320</v>
+      </c>
+      <c r="B13">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1">
+        <v>42700</v>
+      </c>
+      <c r="F13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G13" t="s">
+        <v>329</v>
+      </c>
+      <c r="H13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" t="s">
+        <v>331</v>
+      </c>
+      <c r="J13" t="s">
+        <v>330</v>
+      </c>
+      <c r="K13" t="s">
+        <v>340</v>
+      </c>
+      <c r="L13" t="s">
+        <v>335</v>
+      </c>
+      <c r="M13" t="s">
+        <v>56</v>
+      </c>
+      <c r="N13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>321</v>
+      </c>
+      <c r="B14">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1">
+        <v>42707</v>
+      </c>
+      <c r="F14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" t="s">
+        <v>331</v>
+      </c>
+      <c r="K14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L14" t="s">
+        <v>353</v>
+      </c>
+      <c r="M14" t="s">
+        <v>354</v>
+      </c>
+      <c r="N14" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>322</v>
+      </c>
+      <c r="B15">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1">
+        <v>42714</v>
+      </c>
+      <c r="F15" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" t="s">
+        <v>356</v>
+      </c>
+      <c r="J15" t="s">
+        <v>342</v>
+      </c>
+      <c r="K15" t="s">
+        <v>329</v>
+      </c>
+      <c r="L15" t="s">
+        <v>331</v>
+      </c>
+      <c r="M15" t="s">
+        <v>337</v>
+      </c>
+      <c r="N15" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>323</v>
+      </c>
+      <c r="B16">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1">
+        <v>42721</v>
+      </c>
+      <c r="F16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G16" t="s">
+        <v>342</v>
+      </c>
+      <c r="H16" t="s">
+        <v>340</v>
+      </c>
+      <c r="I16" t="s">
+        <v>331</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" t="s">
+        <v>73</v>
+      </c>
+      <c r="M16" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>308</v>
+      </c>
+      <c r="B17">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" s="1">
+        <v>42756</v>
+      </c>
+      <c r="F17" t="s">
+        <v>151</v>
+      </c>
+      <c r="G17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" t="s">
+        <v>329</v>
+      </c>
+      <c r="I17" t="s">
+        <v>358</v>
+      </c>
+      <c r="J17" t="s">
+        <v>340</v>
+      </c>
+      <c r="K17" t="s">
+        <v>359</v>
+      </c>
+      <c r="L17" t="s">
+        <v>333</v>
+      </c>
+      <c r="M17" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>360</v>
+      </c>
+      <c r="B18">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>361</v>
+      </c>
+      <c r="E18" s="1">
+        <v>42839</v>
+      </c>
+      <c r="F18" t="s">
+        <v>152</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" t="s">
+        <v>362</v>
+      </c>
+      <c r="L18" t="s">
+        <v>363</v>
+      </c>
+      <c r="M18" t="s">
+        <v>364</v>
+      </c>
+      <c r="N18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>365</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>366</v>
+      </c>
+      <c r="E19" s="1">
+        <v>42644</v>
+      </c>
+      <c r="F19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" t="s">
+        <v>183</v>
+      </c>
+      <c r="I19" t="s">
+        <v>367</v>
+      </c>
+      <c r="J19" t="s">
+        <v>368</v>
+      </c>
+      <c r="K19" t="s">
+        <v>355</v>
+      </c>
+      <c r="L19" t="s">
+        <v>369</v>
+      </c>
+      <c r="M19" t="s">
+        <v>370</v>
+      </c>
+      <c r="N19" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>310</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="1">
+        <v>42608</v>
+      </c>
+      <c r="F20" t="s">
+        <v>152</v>
+      </c>
+      <c r="G20" t="s">
+        <v>341</v>
+      </c>
+      <c r="H20" t="s">
+        <v>372</v>
+      </c>
+      <c r="I20" t="s">
+        <v>343</v>
+      </c>
+      <c r="J20" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>311</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>373</v>
+      </c>
+      <c r="E21" s="1">
+        <v>42677</v>
+      </c>
+      <c r="F21" t="s">
+        <v>152</v>
+      </c>
+      <c r="G21" t="s">
+        <v>374</v>
+      </c>
+      <c r="H21" t="s">
+        <v>375</v>
+      </c>
+      <c r="I21" t="s">
+        <v>376</v>
+      </c>
+      <c r="J21" t="s">
+        <v>377</v>
+      </c>
+      <c r="K21" t="s">
+        <v>378</v>
+      </c>
+      <c r="L21" t="s">
+        <v>379</v>
+      </c>
+      <c r="M21" t="s">
+        <v>380</v>
+      </c>
+      <c r="N21" t="s">
+        <v>381</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F3361F-A3A3-4C6E-BD4E-2CCB2D68713A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2">
+        <v>369</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1">
+        <v>42875</v>
+      </c>
+      <c r="F2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" t="s">
+        <v>333</v>
+      </c>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E3" s="1">
+        <v>42882</v>
+      </c>
+      <c r="F3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" t="s">
+        <v>333</v>
+      </c>
+      <c r="K3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B4">
+        <v>407</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42896</v>
+      </c>
+      <c r="F4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" t="s">
+        <v>331</v>
+      </c>
+      <c r="M4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5">
+        <v>227</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1">
+        <v>42938</v>
+      </c>
+      <c r="F5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" t="s">
+        <v>331</v>
+      </c>
+      <c r="M5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B6">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>296</v>
+      </c>
+      <c r="E6" s="1">
+        <v>42952</v>
+      </c>
+      <c r="F6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>331</v>
+      </c>
+      <c r="I6" t="s">
+        <v>382</v>
+      </c>
+      <c r="J6" t="s">
+        <v>383</v>
+      </c>
+      <c r="K6" t="s">
+        <v>337</v>
+      </c>
+      <c r="L6" t="s">
+        <v>220</v>
+      </c>
+      <c r="M6" t="s">
+        <v>384</v>
+      </c>
+      <c r="N6" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B7">
+        <v>160</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1">
+        <v>42958</v>
+      </c>
+      <c r="F7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" t="s">
+        <v>386</v>
+      </c>
+      <c r="N7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B8">
+        <v>159</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1">
+        <v>42966</v>
+      </c>
+      <c r="F8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" t="s">
+        <v>387</v>
+      </c>
+      <c r="N8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B9">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1">
+        <v>42973</v>
+      </c>
+      <c r="F9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" t="s">
+        <v>359</v>
+      </c>
+      <c r="L9" t="s">
+        <v>388</v>
+      </c>
+      <c r="M9" t="s">
+        <v>334</v>
+      </c>
+      <c r="N9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10">
+        <v>460</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1">
+        <v>42994</v>
+      </c>
+      <c r="F10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>301</v>
+      </c>
+      <c r="B11">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1">
+        <v>43001</v>
+      </c>
+      <c r="F11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" t="s">
+        <v>331</v>
+      </c>
+      <c r="J11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" t="s">
+        <v>349</v>
+      </c>
+      <c r="N11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B12">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E12" s="1">
+        <v>43008</v>
+      </c>
+      <c r="F12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" t="s">
+        <v>390</v>
+      </c>
+      <c r="K12" t="s">
+        <v>382</v>
+      </c>
+      <c r="L12" t="s">
+        <v>80</v>
+      </c>
+      <c r="M12" t="s">
+        <v>391</v>
+      </c>
+      <c r="N12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B13">
+        <v>440</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1">
+        <v>43029</v>
+      </c>
+      <c r="F13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" t="s">
+        <v>383</v>
+      </c>
+      <c r="J13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" t="s">
+        <v>55</v>
+      </c>
+      <c r="N13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B14">
+        <v>235</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1">
+        <v>43057</v>
+      </c>
+      <c r="F14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" t="s">
+        <v>329</v>
+      </c>
+      <c r="J14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" t="s">
+        <v>393</v>
+      </c>
+      <c r="L14" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" t="s">
+        <v>75</v>
+      </c>
+      <c r="N14" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>306</v>
+      </c>
+      <c r="B15">
+        <v>164</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1">
+        <v>43085</v>
+      </c>
+      <c r="F15" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>307</v>
+      </c>
+      <c r="B16">
+        <v>154</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1">
+        <v>43120</v>
+      </c>
+      <c r="F16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" t="s">
+        <v>329</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" t="s">
+        <v>48</v>
+      </c>
+      <c r="M16" t="s">
+        <v>138</v>
+      </c>
+      <c r="N16" t="s">
+        <v>359</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1318,7 +3273,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView zoomScale="71" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>